<commit_message>
Added gitignore and updated hours worked.
</commit_message>
<xml_diff>
--- a/Hours Worked/HoursWorked.xlsx
+++ b/Hours Worked/HoursWorked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\University\HonoursProject\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F400D29-6E80-421D-897D-010E2A50167E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B8D3FB-F8A4-4F53-902B-32BD90F5657D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Finishing the SDP and both the review templates and creating this sheet</t>
+  </si>
+  <si>
+    <t>Starting the requirements spec and setting up github boards.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:G501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
       </c>
       <c r="G2">
         <f>SUM(E:E)</f>
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -540,10 +543,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>44160</v>
+      </c>
+      <c r="B7" s="6">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>